<commit_message>
Actualización archivo de extensiones
</commit_message>
<xml_diff>
--- a/Documentación/Extenciones.xlsx
+++ b/Documentación/Extenciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SC_701_ProyectoFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SC_701_ProyectoFinal\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC69E4C-5FF3-4E8C-8856-8BEFCDE5A213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64918EFD-3412-4713-A649-97419F983623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{468FD89D-2680-4636-9B98-934E7B698109}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{468FD89D-2680-4636-9B98-934E7B698109}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,12 +107,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -211,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +523,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>